<commit_message>
Added printing of logwork results and if it is not possible
</commit_message>
<xml_diff>
--- a/Timebooking.xlsx
+++ b/Timebooking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF9E2D9-CF50-4236-8EC5-2EC81AEA23B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB1389E-77DD-4A71-8029-A8C3969E90F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12288" yWindow="516" windowWidth="9852" windowHeight="9948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="2556" windowWidth="9852" windowHeight="9948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>JIRAIssue</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>JIRAURL</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>http://jira.example.com</t>
   </si>
   <si>
     <t>TEST-1</t>
@@ -38,10 +47,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,13 +81,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -349,31 +370,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43674</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{784E4413-E0B7-49DC-8F83-25101D872454}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Functionality to add Comment to Worklog
</commit_message>
<xml_diff>
--- a/Timebooking.xlsx
+++ b/Timebooking.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB1389E-77DD-4A71-8029-A8C3969E90F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="2556" windowWidth="9852" windowHeight="9948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="2556" windowWidth="9852" windowHeight="9948"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>JIRAIssue</t>
   </si>
@@ -34,19 +36,25 @@
     <t>JIRAURL</t>
   </si>
   <si>
-    <t>3h</t>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Testcomment</t>
   </si>
   <si>
     <t>http://jira.example.com</t>
   </si>
   <si>
-    <t>TEST-1</t>
+    <t>TST-1</t>
+  </si>
+  <si>
+    <t>2h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,20 +377,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -395,24 +404,31 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43675</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43674</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{784E4413-E0B7-49DC-8F83-25101D872454}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>